<commit_message>
supports multiple LSA & machines
</commit_message>
<xml_diff>
--- a/apidev/jobdata.xlsx
+++ b/apidev/jobdata.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\BTP2\apidev\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11115" windowHeight="3480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14850" windowHeight="5985"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -914,7 +910,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,7 +950,7 @@
         <v>11</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>12</v>
@@ -977,7 +973,7 @@
         <v>22</v>
       </c>
       <c r="B3">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -1000,7 +996,7 @@
         <v>33</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>45</v>
@@ -1023,7 +1019,7 @@
         <v>44</v>
       </c>
       <c r="B5">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>34</v>
@@ -1046,7 +1042,7 @@
         <v>55</v>
       </c>
       <c r="B6">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <v>65</v>
@@ -1069,7 +1065,7 @@
         <v>66</v>
       </c>
       <c r="B7">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <v>76</v>
@@ -1092,7 +1088,7 @@
         <v>77</v>
       </c>
       <c r="B8">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <v>23</v>
@@ -1115,7 +1111,7 @@
         <v>88</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <v>21</v>
@@ -1138,7 +1134,7 @@
         <v>99</v>
       </c>
       <c r="B10">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>32</v>
@@ -1161,7 +1157,7 @@
         <v>1010</v>
       </c>
       <c r="B11">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C11">
         <v>12</v>

</xml_diff>

<commit_message>
1. BugFix for job start time 2. Added penalty per unit time for jobs getProcessingTime() in job should return values in milliseconds for consistency but since used in B&B, I'ven't changed it.
</commit_message>
<xml_diff>
--- a/apidev/jobdata.xlsx
+++ b/apidev/jobdata.xlsx
@@ -9,13 +9,13 @@
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
   <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>id</t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>Due Date (Seconds)</t>
+  </si>
+  <si>
+    <t>Penalty Rate</t>
+  </si>
+  <si>
+    <t>Cost</t>
   </si>
 </sst>
 </file>
@@ -615,7 +621,11 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -629,16 +639,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G11" totalsRowShown="0">
-  <autoFilter ref="A1:G11"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I11" totalsRowShown="0">
+  <autoFilter ref="A1:I11"/>
+  <tableColumns count="9">
     <tableColumn id="1" name="id"/>
-    <tableColumn id="2" name="Process.time (Seconds)"/>
+    <tableColumn id="2" name="Process.time (Seconds)" dataDxfId="0"/>
     <tableColumn id="3" name="quantity"/>
     <tableColumn id="4" name="Dimensions"/>
     <tableColumn id="5" name="Attributes"/>
     <tableColumn id="6" name="CPN"/>
     <tableColumn id="7" name="Due Date (Seconds)"/>
+    <tableColumn id="8" name="Penalty Rate"/>
+    <tableColumn id="9" name="Cost"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -907,10 +919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,7 +934,7 @@
     <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -944,13 +956,19 @@
       <c r="G1" t="s">
         <v>22</v>
       </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C2">
         <v>12</v>
@@ -965,15 +983,21 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>40</v>
+        <v>22</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>22</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -988,15 +1012,21 @@
         <v>2</v>
       </c>
       <c r="G3">
-        <v>30</v>
+        <v>22</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>33</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C4">
         <v>45</v>
@@ -1011,15 +1041,21 @@
         <v>3</v>
       </c>
       <c r="G4">
-        <v>50</v>
+        <v>22</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>44</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C5">
         <v>34</v>
@@ -1034,15 +1070,21 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>55</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C6">
         <v>65</v>
@@ -1057,15 +1099,21 @@
         <v>2</v>
       </c>
       <c r="G6">
-        <v>50</v>
+        <v>22</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>66</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C7">
         <v>76</v>
@@ -1080,15 +1128,21 @@
         <v>2</v>
       </c>
       <c r="G7">
-        <v>18</v>
+        <v>22</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>77</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C8">
         <v>23</v>
@@ -1103,15 +1157,21 @@
         <v>1</v>
       </c>
       <c r="G8">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>88</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C9">
         <v>21</v>
@@ -1126,15 +1186,21 @@
         <v>2</v>
       </c>
       <c r="G9">
-        <v>10</v>
+        <v>22</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>99</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C10">
         <v>32</v>
@@ -1149,15 +1215,21 @@
         <v>3</v>
       </c>
       <c r="G10">
-        <v>30</v>
+        <v>22</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1010</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C11">
         <v>12</v>
@@ -1172,7 +1244,13 @@
         <v>2</v>
       </c>
       <c r="G11">
-        <v>40</v>
+        <v>22</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
supports reply with feature of ACL message
WARNING : Change in ZoneDataUpdate class. All files where it was used
has been modified

Remaining BUG: wrong processing time
</commit_message>
<xml_diff>
--- a/apidev/jobdata.xlsx
+++ b/apidev/jobdata.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\BTP2_new\apidev\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14850" windowHeight="5985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14670" windowHeight="5985"/>
   </bookViews>
   <sheets>
     <sheet name="job1" sheetId="1" r:id="rId1"/>
@@ -24,6 +19,7 @@
     <sheet name="job10" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:K17"/>
 </workbook>
 </file>
 
@@ -1126,7 +1122,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
job operation read bug removal
</commit_message>
<xml_diff>
--- a/apidev/jobdata.xlsx
+++ b/apidev/jobdata.xlsx
@@ -3,11 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\MAS-GUI\AgentProxy\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14670" windowHeight="5985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14850" windowHeight="5985" activeTab="9"/>
   </bookViews>
   <sheets>
-    <sheet name="job1" sheetId="1" r:id="rId1"/>
+    <sheet name="job1" sheetId="11" r:id="rId1"/>
     <sheet name="job2" sheetId="2" r:id="rId2"/>
     <sheet name="job3" sheetId="3" r:id="rId3"/>
     <sheet name="job4" sheetId="4" r:id="rId4"/>
@@ -19,12 +24,11 @@
     <sheet name="job10" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K17"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
@@ -36,9 +40,6 @@
   </si>
   <si>
     <t>Attributes</t>
-  </si>
-  <si>
-    <t>10,23</t>
   </si>
   <si>
     <t>A2</t>
@@ -62,19 +63,16 @@
     <t>Processing Times</t>
   </si>
   <si>
-    <t>operation1</t>
+    <t>Penalty Rate</t>
   </si>
   <si>
-    <t>Penalty</t>
+    <t>Operation_1</t>
   </si>
   <si>
-    <t>operation2</t>
+    <t>Operation_2</t>
   </si>
   <si>
-    <t>9,12</t>
-  </si>
-  <si>
-    <t>operation3</t>
+    <t>Operation_3</t>
   </si>
 </sst>
 </file>
@@ -564,9 +562,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="33" borderId="3" xfId="4" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -627,7 +624,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D6" totalsRowShown="0" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Table126" displayName="Table126" ref="A1:D6" totalsRowShown="0" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4">
   <autoFilter ref="A1:D6"/>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
@@ -643,7 +640,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table312" displayName="Table312" ref="E1:E2" totalsRowShown="0">
   <autoFilter ref="E1:E2"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Penalty"/>
+    <tableColumn id="1" name="Penalty Rate"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -666,7 +663,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table314" displayName="Table314" ref="E1:E2" totalsRowShown="0">
   <autoFilter ref="E1:E2"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Penalty"/>
+    <tableColumn id="1" name="Penalty Rate"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -689,7 +686,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table316" displayName="Table316" ref="E1:E2" totalsRowShown="0">
   <autoFilter ref="E1:E2"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Penalty"/>
+    <tableColumn id="1" name="Penalty Rate"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -712,7 +709,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table318" displayName="Table318" ref="E1:E2" totalsRowShown="0">
   <autoFilter ref="E1:E2"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Penalty"/>
+    <tableColumn id="1" name="Penalty Rate"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -735,7 +732,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table320" displayName="Table320" ref="E1:E2" totalsRowShown="0">
   <autoFilter ref="E1:E2"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Penalty"/>
+    <tableColumn id="1" name="Penalty Rate"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -755,10 +752,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="E1:E2" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Table327" displayName="Table327" ref="E1:E2" totalsRowShown="0">
   <autoFilter ref="E1:E2"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Penalty"/>
+    <tableColumn id="1" name="Penalty Rate"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -768,7 +765,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table322" displayName="Table322" ref="E1:E2" totalsRowShown="0">
   <autoFilter ref="E1:E2"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Penalty"/>
+    <tableColumn id="1" name="Penalty Rate"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -791,7 +788,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table36" displayName="Table36" ref="E1:E2" totalsRowShown="0">
   <autoFilter ref="E1:E2"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Penalty"/>
+    <tableColumn id="1" name="Penalty Rate"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -814,7 +811,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table38" displayName="Table38" ref="E1:E2" totalsRowShown="0">
   <autoFilter ref="E1:E2"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Penalty"/>
+    <tableColumn id="1" name="Penalty Rate"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -837,7 +834,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table310" displayName="Table310" ref="E1:E2" totalsRowShown="0">
   <autoFilter ref="E1:E2"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Penalty"/>
+    <tableColumn id="1" name="Penalty Rate"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1119,10 +1116,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,7 +1128,7 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1142,13 +1139,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1165,20 +1162,20 @@
         <v>10</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1189,30 +1186,30 @@
       <c r="B4">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
+      <c r="C5">
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -1221,17 +1218,8 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E10" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="1"/>
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1246,8 +1234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,7 +1244,7 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1267,13 +1255,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1290,20 +1278,20 @@
         <v>2</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1314,30 +1302,30 @@
       <c r="B4">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
+      <c r="C5">
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -1346,7 +1334,7 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1363,7 +1351,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1372,7 +1360,7 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1383,13 +1371,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1406,20 +1394,20 @@
         <v>2</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1430,16 +1418,16 @@
       <c r="B4">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>9</v>
@@ -1448,7 +1436,7 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1465,7 +1453,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1474,7 +1462,7 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1485,13 +1473,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1512,16 +1500,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1532,11 +1520,11 @@
       <c r="B4">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1553,7 +1541,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1562,7 +1550,7 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1573,13 +1561,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1600,16 +1588,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1620,25 +1608,25 @@
       <c r="B4">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
+      <c r="C5">
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1655,7 +1643,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D16:D17"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1664,7 +1652,7 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1675,13 +1663,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1698,20 +1686,20 @@
         <v>2</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1722,30 +1710,30 @@
       <c r="B4">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
+      <c r="C5">
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -1754,7 +1742,7 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1771,7 +1759,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1780,7 +1768,7 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1791,13 +1779,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1818,16 +1806,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1838,25 +1826,25 @@
       <c r="B4">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>21</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
+      <c r="C5">
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1873,7 +1861,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1882,7 +1870,7 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1893,13 +1881,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1916,35 +1904,35 @@
         <v>2</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1961,7 +1949,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1970,7 +1958,7 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1981,13 +1969,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2008,16 +1996,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2028,30 +2016,30 @@
       <c r="B4">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
+      <c r="C5">
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -2060,7 +2048,7 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -2077,7 +2065,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2086,7 +2074,7 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2097,13 +2085,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2120,49 +2108,49 @@
         <v>2</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
+      <c r="C5">
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>